<commit_message>
update code to member
</commit_message>
<xml_diff>
--- a/window.xlsx
+++ b/window.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -1449,6 +1449,646 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 5.96 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G26" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H26" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 6.18 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G27" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H27" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 6.15 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G28" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H28" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 6.10 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G29" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H29" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 6.33 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G30" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H30" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 5.49 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G31" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H31" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 5.81 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G32" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H32" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 5.64 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G33" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H33" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 6.24 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G34" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H34" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 6.24 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G35" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H35" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 6.24 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G36" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H36" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 6.26 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G37" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H37" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 5.71 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G38" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H38" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 7.50 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G39" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H39" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 7.55 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G40" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H40" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 5.84 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G41" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H41" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update code to git
</commit_message>
<xml_diff>
--- a/window.xlsx
+++ b/window.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -2329,6 +2329,46 @@
         </is>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="inlineStr">
+        <is>
+          <t>Total Memory: 15.86 GB, Used Memory: 7.47 GB, Total Disk Space: 237.84 GB</t>
+        </is>
+      </c>
+      <c r="C48" s="2" t="inlineStr">
+        <is>
+          <t>Sovan.Souern</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>1L0N1W2</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>AMD64</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="G48" s="2" t="inlineStr">
+        <is>
+          <t>PNCL114</t>
+        </is>
+      </c>
+      <c r="H48" s="2" t="inlineStr">
+        <is>
+          <t>AT/AT COMPATIBLE</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>